<commit_message>
Ranking System function added
</commit_message>
<xml_diff>
--- a/computer_science.xlsx
+++ b/computer_science.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AS11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FGHIJK633839</t>
+          <t>BCDEFG474849</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -592,60 +592,702 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" t="n">
+        <v>49</v>
+      </c>
+      <c r="G2" t="n">
+        <v>47</v>
+      </c>
+      <c r="H2" t="n">
+        <v>81</v>
+      </c>
+      <c r="J2" t="n">
+        <v>87</v>
+      </c>
+      <c r="N2" t="n">
+        <v>10</v>
+      </c>
+      <c r="O2" t="n">
+        <v>10</v>
+      </c>
+      <c r="R2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO2" t="n">
+        <v>33</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>57</v>
+      </c>
+      <c r="AR2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DEFGHI141516</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>23</v>
+      </c>
+      <c r="F3" t="n">
+        <v>87</v>
+      </c>
+      <c r="G3" t="n">
+        <v>80</v>
+      </c>
+      <c r="H3" t="n">
+        <v>89</v>
+      </c>
+      <c r="I3" t="n">
+        <v>66</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO3" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>71</v>
+      </c>
+      <c r="AR3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PEFGHI202122</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>84</v>
+      </c>
+      <c r="G4" t="n">
+        <v>55</v>
+      </c>
+      <c r="H4" t="n">
+        <v>73</v>
+      </c>
+      <c r="J4" t="n">
+        <v>75</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO4" t="n">
+        <v>35</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>73</v>
+      </c>
+      <c r="AR4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ABCDEF373839</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>27</v>
+      </c>
+      <c r="F5" t="n">
+        <v>62</v>
+      </c>
+      <c r="G5" t="n">
+        <v>79</v>
+      </c>
+      <c r="H5" t="n">
+        <v>55</v>
+      </c>
+      <c r="K5" t="n">
+        <v>77</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>52</v>
+      </c>
+      <c r="AR5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>UVWX373839</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F6" t="n">
+        <v>81</v>
+      </c>
+      <c r="G6" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" t="n">
+        <v>74</v>
+      </c>
+      <c r="I6" t="n">
+        <v>93</v>
+      </c>
+      <c r="N6" t="n">
+        <v>10</v>
+      </c>
+      <c r="O6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO6" t="n">
+        <v>43</v>
+      </c>
+      <c r="AP6" t="n">
         <v>18</v>
       </c>
-      <c r="F2" t="n">
+      <c r="AQ6" t="n">
+        <v>82</v>
+      </c>
+      <c r="AR6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GHIJKL272829</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18</v>
+      </c>
+      <c r="F7" t="n">
+        <v>92</v>
+      </c>
+      <c r="G7" t="n">
+        <v>84</v>
+      </c>
+      <c r="H7" t="n">
+        <v>77</v>
+      </c>
+      <c r="M7" t="n">
+        <v>94</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO7" t="n">
+        <v>43</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>18</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>81</v>
+      </c>
+      <c r="AR7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MNOPQR373839</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26</v>
+      </c>
+      <c r="F8" t="n">
+        <v>51</v>
+      </c>
+      <c r="G8" t="n">
+        <v>66</v>
+      </c>
+      <c r="H8" t="n">
+        <v>57</v>
+      </c>
+      <c r="K8" t="n">
         <v>97</v>
       </c>
-      <c r="G2" t="n">
-        <v>59</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="N8" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" t="n">
+        <v>10</v>
+      </c>
+      <c r="R8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>19</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>71</v>
+      </c>
+      <c r="AR8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>OPQRST242526</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>27</v>
+      </c>
+      <c r="F9" t="n">
+        <v>70</v>
+      </c>
+      <c r="G9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H9" t="n">
+        <v>94</v>
+      </c>
+      <c r="L9" t="n">
+        <v>81</v>
+      </c>
+      <c r="N9" t="n">
+        <v>8</v>
+      </c>
+      <c r="O9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>9</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO9" t="n">
+        <v>38</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>24</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>84</v>
+      </c>
+      <c r="AR9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OPQRST525354</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>18</v>
+      </c>
+      <c r="F10" t="n">
+        <v>61</v>
+      </c>
+      <c r="G10" t="n">
         <v>75</v>
       </c>
-      <c r="K2" t="n">
-        <v>69</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="H10" t="n">
+        <v>78</v>
+      </c>
+      <c r="M10" t="n">
+        <v>53</v>
+      </c>
+      <c r="N10" t="n">
+        <v>7</v>
+      </c>
+      <c r="O10" t="n">
+        <v>10</v>
+      </c>
+      <c r="R10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK10" t="n">
         <v>8</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AO10" t="n">
+        <v>33</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>70</v>
+      </c>
+      <c r="AR10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MNOPQR151617</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>26</v>
+      </c>
+      <c r="F11" t="n">
+        <v>58</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>52</v>
+      </c>
+      <c r="L11" t="n">
+        <v>66</v>
+      </c>
+      <c r="N11" t="n">
         <v>7</v>
       </c>
-      <c r="AC2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD2" t="n">
+      <c r="O11" t="n">
+        <v>10</v>
+      </c>
+      <c r="R11" t="n">
         <v>6</v>
       </c>
-      <c r="AJ2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AC11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL11" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
-      <c r="AO2" t="n">
-        <v>37</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>30</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>83</v>
-      </c>
-      <c r="AR2" t="b">
-        <v>1</v>
+      <c r="AO11" t="n">
+        <v>34</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>72</v>
+      </c>
+      <c r="AR11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
admission_satus fucntion properly working
</commit_message>
<xml_diff>
--- a/computer_science.xlsx
+++ b/computer_science.xlsx
@@ -583,40 +583,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BCDEFG474849</t>
+          <t>GHIJK464748</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>male</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" t="n">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="G2" t="n">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="H2" t="n">
-        <v>81</v>
-      </c>
-      <c r="J2" t="n">
-        <v>87</v>
+        <v>95</v>
+      </c>
+      <c r="K2" t="n">
+        <v>78</v>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="R2" t="n">
         <v>7</v>
@@ -625,36 +625,39 @@
         <v>10</v>
       </c>
       <c r="AD2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AI2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN2" t="n">
+        <v>19</v>
+      </c>
       <c r="AO2" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="AP2" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AQ2" t="n">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="AR2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DEFGHI141516</t>
+          <t>LMNOPQ606162</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -666,66 +669,69 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>23</v>
       </c>
       <c r="F3" t="n">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="G3" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H3" t="n">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I3" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="N3" t="n">
         <v>10</v>
       </c>
       <c r="O3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ3" t="n">
         <v>9</v>
       </c>
-      <c r="AC3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>10</v>
-      </c>
       <c r="AL3" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN3" t="n">
+        <v>18</v>
+      </c>
       <c r="AO3" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AP3" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AQ3" t="n">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="AR3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PEFGHI202122</t>
+          <t>DEFGHI656667</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -737,39 +743,39 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="G4" t="n">
+        <v>74</v>
+      </c>
+      <c r="H4" t="n">
         <v>55</v>
       </c>
-      <c r="H4" t="n">
-        <v>73</v>
-      </c>
       <c r="J4" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="N4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O4" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="R4" t="n">
+        <v>7</v>
       </c>
       <c r="AC4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AI4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ4" t="n">
         <v>10</v>
       </c>
       <c r="AL4" t="inlineStr">
@@ -777,26 +783,29 @@
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN4" t="n">
+        <v>19</v>
+      </c>
       <c r="AO4" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AP4" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="AQ4" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AR4" t="b">
         <v>1</v>
       </c>
       <c r="AS4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ABCDEF373839</t>
+          <t>KLDEFG434445</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -808,66 +817,69 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G5" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
-      </c>
-      <c r="K5" t="n">
+        <v>65</v>
+      </c>
+      <c r="L5" t="n">
         <v>77</v>
       </c>
       <c r="N5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q5" t="n">
         <v>7</v>
       </c>
       <c r="AC5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AK5" t="n">
         <v>10</v>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
+      </c>
+      <c r="AN5" t="n">
+        <v>18</v>
       </c>
       <c r="AO5" t="n">
         <v>34</v>
       </c>
       <c r="AP5" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="AQ5" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="AR5" t="b">
         <v>0</v>
       </c>
       <c r="AS5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UVWX373839</t>
+          <t>DEFGHI838485</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -882,63 +894,66 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G6" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="H6" t="n">
-        <v>74</v>
-      </c>
-      <c r="I6" t="n">
-        <v>93</v>
+        <v>55</v>
+      </c>
+      <c r="L6" t="n">
+        <v>94</v>
       </c>
       <c r="N6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q6" t="n">
+        <v>6</v>
+      </c>
+      <c r="R6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI6" t="n">
         <v>8</v>
       </c>
-      <c r="AC6" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>8</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>7</v>
-      </c>
       <c r="AL6" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN6" t="n">
+        <v>16</v>
+      </c>
       <c r="AO6" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="AP6" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AQ6" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="AR6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GHIJKL272829</t>
+          <t>HIJKLM757677</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -947,69 +962,72 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G7" t="n">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H7" t="n">
         <v>77</v>
       </c>
-      <c r="M7" t="n">
-        <v>94</v>
+      <c r="L7" t="n">
+        <v>54</v>
       </c>
       <c r="N7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN7" t="n">
+        <v>12</v>
+      </c>
       <c r="AO7" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="AP7" t="n">
         <v>18</v>
       </c>
       <c r="AQ7" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="AR7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MNOPQR373839</t>
+          <t>DLMNOP808182</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1021,66 +1039,69 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F8" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="G8" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H8" t="n">
-        <v>57</v>
-      </c>
-      <c r="K8" t="n">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="M8" t="n">
+        <v>68</v>
       </c>
       <c r="N8" t="n">
+        <v>7</v>
+      </c>
+      <c r="O8" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD8" t="n">
         <v>8</v>
       </c>
-      <c r="O8" t="n">
-        <v>10</v>
-      </c>
-      <c r="R8" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>7</v>
+      <c r="AJ8" t="n">
+        <v>10</v>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
           <t>Computer science</t>
         </is>
       </c>
+      <c r="AN8" t="n">
+        <v>21</v>
+      </c>
       <c r="AO8" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AP8" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AQ8" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AR8" t="b">
         <v>1</v>
       </c>
       <c r="AS8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>OPQRST242526</t>
+          <t>FGHI121314</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1095,63 +1116,66 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" t="n">
+        <v>94</v>
+      </c>
+      <c r="G9" t="n">
+        <v>52</v>
+      </c>
+      <c r="H9" t="n">
+        <v>93</v>
+      </c>
+      <c r="L9" t="n">
+        <v>87</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7</v>
+      </c>
+      <c r="O9" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AN9" t="n">
+        <v>18</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ9" t="n">
         <v>70</v>
       </c>
-      <c r="G9" t="n">
-        <v>60</v>
-      </c>
-      <c r="H9" t="n">
-        <v>94</v>
-      </c>
-      <c r="L9" t="n">
-        <v>81</v>
-      </c>
-      <c r="N9" t="n">
-        <v>8</v>
-      </c>
-      <c r="O9" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>9</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>9</v>
-      </c>
-      <c r="AL9" t="inlineStr">
-        <is>
-          <t>Computer science</t>
-        </is>
-      </c>
-      <c r="AO9" t="n">
-        <v>38</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>24</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>84</v>
-      </c>
       <c r="AR9" t="b">
         <v>1</v>
       </c>
       <c r="AS9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OPQRST525354</t>
+          <t>NOP959697</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1160,69 +1184,72 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" t="n">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G10" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="H10" t="n">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="M10" t="n">
+        <v>47</v>
+      </c>
+      <c r="N10" t="n">
+        <v>10</v>
+      </c>
+      <c r="O10" t="n">
+        <v>8</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AN10" t="n">
+        <v>16</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ10" t="n">
         <v>53</v>
       </c>
-      <c r="N10" t="n">
-        <v>7</v>
-      </c>
-      <c r="O10" t="n">
-        <v>10</v>
-      </c>
-      <c r="R10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>7</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL10" t="inlineStr">
-        <is>
-          <t>Computer science</t>
-        </is>
-      </c>
-      <c r="AO10" t="n">
-        <v>33</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>20</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>70</v>
-      </c>
       <c r="AR10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MNOPQR151617</t>
+          <t>FGFGHI314151</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1234,60 +1261,63 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" t="n">
+        <v>65</v>
+      </c>
+      <c r="G11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H11" t="n">
+        <v>83</v>
+      </c>
+      <c r="L11" t="n">
+        <v>99</v>
+      </c>
+      <c r="N11" t="n">
+        <v>10</v>
+      </c>
+      <c r="O11" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>Computer science</t>
+        </is>
+      </c>
+      <c r="AN11" t="n">
+        <v>18</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ11" t="n">
         <v>58</v>
       </c>
-      <c r="G11" t="n">
-        <v>100</v>
-      </c>
-      <c r="H11" t="n">
-        <v>52</v>
-      </c>
-      <c r="L11" t="n">
-        <v>66</v>
-      </c>
-      <c r="N11" t="n">
-        <v>7</v>
-      </c>
-      <c r="O11" t="n">
-        <v>10</v>
-      </c>
-      <c r="R11" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>6</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>7</v>
-      </c>
-      <c r="AL11" t="inlineStr">
-        <is>
-          <t>Computer science</t>
-        </is>
-      </c>
-      <c r="AO11" t="n">
-        <v>34</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>20</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>72</v>
-      </c>
       <c r="AR11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>